<commit_message>
tablas de la encuesta
</commit_message>
<xml_diff>
--- a/ENCUESTA/Resultado_encuesta - copia.xlsx
+++ b/ENCUESTA/Resultado_encuesta - copia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mercedes_Soriano\Desktop\tesis2018-master\tesis2018-master\ENCUESTA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plataformavirtual.NUR.000\Desktop\tesis\ENCUESTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -384,15 +384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -407,6 +398,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,20 +690,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E104" sqref="E104"/>
+      <selection pane="topRight" activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="9"/>
-    <col min="2" max="2" width="50.7109375" style="9" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="9"/>
+    <col min="1" max="1" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="50.7109375" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -823,7 +823,7 @@
       </c>
     </row>
     <row r="2" spans="1:75" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -938,7 +938,7 @@
       </c>
     </row>
     <row r="3" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1146,12 +1146,12 @@
         <v>1</v>
       </c>
       <c r="BW3" s="3">
-        <f t="shared" ref="BW3:BW19" si="0">SUM(B3:BV3)</f>
+        <f t="shared" ref="BW3:BW18" si="0">SUM(B3:BV3)</f>
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:75" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
     </row>
     <row r="5" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1305,7 +1305,7 @@
       </c>
     </row>
     <row r="6" spans="1:75" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1393,7 +1393,7 @@
       </c>
     </row>
     <row r="7" spans="1:75" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
     </row>
     <row r="8" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1577,7 +1577,7 @@
       </c>
     </row>
     <row r="9" spans="1:75" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
     </row>
     <row r="10" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1788,7 +1788,7 @@
       </c>
     </row>
     <row r="11" spans="1:75" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
     </row>
     <row r="12" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1972,7 +1972,7 @@
       </c>
     </row>
     <row r="13" spans="1:75" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="14" spans="1:75" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -2109,7 +2109,7 @@
       </c>
     </row>
     <row r="15" spans="1:75" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2151,7 +2151,7 @@
       </c>
     </row>
     <row r="16" spans="1:75" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2188,7 +2188,7 @@
       </c>
     </row>
     <row r="17" spans="1:75" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="18" spans="1:75" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2327,613 +2327,613 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:75" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:75" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Z19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AQ19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AT19" s="8">
-        <v>1</v>
-      </c>
-      <c r="BW19" s="8">
+      <c r="Z19" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ19" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BW19" s="5">
         <f>SUM(B19:BV19)</f>
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="9">
+      <c r="B25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
         <v>184</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="6">
         <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="6">
         <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:75" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="6">
         <v>2</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="6">
         <v>313</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="6">
         <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="6">
         <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="6">
         <v>3</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="6">
         <v>8</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="6">
         <f>SUM(C37:C40)</f>
         <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="6">
         <v>4</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="6">
         <v>174</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="6">
         <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="6">
         <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="6">
         <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="6">
         <v>5</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="6">
         <v>232</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="6">
         <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="6">
         <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="6">
         <v>6</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="6">
         <v>218</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="6">
         <v>341</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="6">
         <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="A62" s="6">
         <v>7</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C64" s="6">
         <v>144</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G64" s="9">
+      <c r="G64" s="6">
         <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C65" s="6">
         <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="6">
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
         <v>8</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C71" s="9">
+      <c r="C71" s="6">
         <v>5</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="6">
         <f>SUM(C71:C95)</f>
         <v>341</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C72" s="6">
         <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C73" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C74" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C77" s="9">
+      <c r="C77" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C78" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C79" s="9">
+      <c r="C79" s="6">
         <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C80" s="9">
+      <c r="C80" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C81" s="9">
+      <c r="C81" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C82" s="9">
+      <c r="C82" s="6">
         <v>94</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="12" t="s">
+      <c r="B83" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C83" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C84" s="9">
+      <c r="C84" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C85" s="9">
+      <c r="C85" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C86" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="12" t="s">
+      <c r="B87" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C87" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="12" t="s">
+      <c r="B88" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C88" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B90" s="12" t="s">
+      <c r="B90" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="12" t="s">
+      <c r="B91" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B92" s="12" t="s">
+      <c r="B92" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="12" t="s">
+      <c r="B94" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="12" t="s">
+      <c r="B95" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="9">
+      <c r="A98" s="6">
         <v>7</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B98" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F98" s="9" t="s">
+      <c r="F98" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G98" s="9">
+      <c r="G98" s="6">
         <f>SUM(C100:C104)</f>
         <v>341</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="6">
         <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
+      <c r="A101" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="6">
         <v>52</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B102" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="6">
         <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="9" t="s">
+      <c r="B103" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C103" s="6">
         <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="6">
         <v>32</v>
       </c>
     </row>

</xml_diff>